<commit_message>
Third commit for Selenium Java automation code
</commit_message>
<xml_diff>
--- a/target/test-classes/testdata/testdata.xlsx
+++ b/target/test-classes/testdata/testdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\eclipse-workspace\SeleniumAutomationFramework\TestAutomationFramework\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28CF2BF5-F8A2-437C-BEC3-79E9FD70CFE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C9C7CDD-02C3-4233-AC47-C67519D690EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="11">
   <si>
     <t>username</t>
   </si>
@@ -55,13 +55,19 @@
     <t>correct_password</t>
   </si>
   <si>
-    <t>status</t>
-  </si>
-  <si>
     <t>failed</t>
   </si>
   <si>
     <t>passed</t>
+  </si>
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>Status</t>
   </si>
 </sst>
 </file>
@@ -442,7 +448,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -453,13 +459,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -470,7 +476,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -481,7 +487,7 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -492,7 +498,7 @@
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -503,7 +509,7 @@
         <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>